<commit_message>
2019-01-08 15:02:00 meizi asus
</commit_message>
<xml_diff>
--- a/PhoneInfoServerIIS/Dev/Record.xlsx
+++ b/PhoneInfoServerIIS/Dev/Record.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\C\PhoneInfoServerIIS\PhoneInfoServerIIS\Dev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\工作文档\老秦项目\荆州项目\PhoneInfoServerIIS\PhoneInfoServerIIS\Dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC799DE2-6060-40EE-9F78-329213E18941}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C24619-26EE-49BC-B8E7-6B75BA57A908}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12915" windowHeight="9285" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="186">
   <si>
     <t>项目</t>
   </si>
@@ -691,6 +691,22 @@
   </si>
   <si>
     <t>上传测试组信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AddSysModule</t>
+  </si>
+  <si>
+    <t>DeleteSysModule</t>
+  </si>
+  <si>
+    <t>UpdateSysModule</t>
+  </si>
+  <si>
+    <t>GetSysModule</t>
+  </si>
+  <si>
+    <t>增删改查 系统查询模板</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -760,7 +776,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -807,13 +823,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -861,9 +886,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1855,10 +1883,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC083895-FA8B-4D2D-BD04-6F2A2AF7FA97}">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2452,7 +2480,36 @@
         <v>180</v>
       </c>
     </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A33" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A34" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="B34" s="17"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A35" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B35" s="17"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A36" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="B36" s="17"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B33:B36"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="G26" r:id="rId1" xr:uid="{12E139AF-E3B9-40B0-BFDC-B8A4B74E82B5}"/>

</xml_diff>